<commit_message>
Fix data issues for debt worries over time in excel. Updated chapter with more text, better visual spacing
</commit_message>
<xml_diff>
--- a/data/ucues_alluc.xlsx
+++ b/data/ucues_alluc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanolan\OneDrive\IR_Folder\UCSD_Gaps_git\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanolan\OneDrive\IR_Folder\UCSD_Gaps_Quarto\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0FD69F7-E2DE-46E3-9C52-1893E2990FDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA7AE82-A25E-4BE5-960C-15E06081C133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1390" yWindow="3690" windowWidth="19200" windowHeight="5180" xr2:uid="{27077269-9732-4CAA-AC77-88FD1CE5D0EE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{27077269-9732-4CAA-AC77-88FD1CE5D0EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1107,8 +1107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8C231E6-8F8A-44F7-8087-CF662AB14A00}">
   <dimension ref="A1:K130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="F131" sqref="F131"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="F112" sqref="F112:J118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1158,194 +1158,212 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2">
+      <c r="D2" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="10">
         <v>2022</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="I2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J2" s="9">
-        <v>0.57999999999999996</v>
+        <v>0.15</v>
+      </c>
+      <c r="K2">
+        <v>8073</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3">
+      <c r="D3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="10">
         <v>2022</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="I3">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J3" s="9">
-        <v>0.56999999999999995</v>
+        <v>0.16</v>
+      </c>
+      <c r="K3">
+        <v>8960</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4">
+      <c r="D4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="10">
         <v>2022</v>
       </c>
       <c r="G4" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="I4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J4" s="9">
-        <v>0.57999999999999996</v>
+        <v>0.15</v>
+      </c>
+      <c r="K4">
+        <v>8330</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5">
+      <c r="D5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="10">
         <v>2022</v>
       </c>
       <c r="G5" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="I5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J5" s="9">
-        <v>0.44</v>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="K5">
+        <v>7830</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6">
+      <c r="D6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="10">
         <v>2022</v>
       </c>
       <c r="G6" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="I6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J6" s="9">
-        <v>0.49</v>
+        <v>0.19</v>
+      </c>
+      <c r="K6">
+        <v>10289</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7">
+      <c r="D7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="10">
         <v>2022</v>
       </c>
       <c r="G7" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="I7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J7" s="9">
-        <v>0.57999999999999996</v>
+        <v>0.2</v>
+      </c>
+      <c r="K7">
+        <v>11043</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1353,7 +1371,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -1365,7 +1383,7 @@
         <v>12</v>
       </c>
       <c r="F8">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="G8" t="s">
         <v>13</v>
@@ -1374,10 +1392,10 @@
         <v>31</v>
       </c>
       <c r="I8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J8" s="9">
-        <v>0.56999999999999995</v>
+        <v>0.65999999999999992</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1385,7 +1403,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
@@ -1397,19 +1415,19 @@
         <v>12</v>
       </c>
       <c r="F9">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="G9" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="6" t="s">
-        <v>31</v>
+      <c r="H9" t="s">
+        <v>25</v>
       </c>
       <c r="I9">
-        <v>3</v>
-      </c>
-      <c r="J9" s="9">
-        <v>0.51</v>
+        <v>1</v>
+      </c>
+      <c r="J9" s="8">
+        <v>0.34</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1417,7 +1435,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
@@ -1429,7 +1447,7 @@
         <v>12</v>
       </c>
       <c r="F10">
-        <v>2018</v>
+        <v>2022</v>
       </c>
       <c r="G10" t="s">
         <v>13</v>
@@ -1441,7 +1459,7 @@
         <v>3</v>
       </c>
       <c r="J10" s="9">
-        <v>0.53</v>
+        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1449,7 +1467,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
         <v>11</v>
@@ -1467,13 +1485,13 @@
         <v>13</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J11" s="9">
-        <v>0.56999999999999995</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1481,7 +1499,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
         <v>11</v>
@@ -1498,22 +1516,22 @@
       <c r="G12" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="6" t="s">
-        <v>31</v>
+      <c r="H12" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="I12">
-        <v>3</v>
-      </c>
-      <c r="J12" s="9">
-        <v>0.64</v>
+        <v>1</v>
+      </c>
+      <c r="J12" s="8">
+        <v>0.24</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
         <v>11</v>
@@ -1528,21 +1546,21 @@
         <v>2020</v>
       </c>
       <c r="G13" t="s">
-        <v>27</v>
-      </c>
-      <c r="H13" t="s">
-        <v>28</v>
+        <v>13</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="I13">
-        <v>1</v>
-      </c>
-      <c r="J13" s="8">
-        <v>0.05</v>
+        <v>2</v>
+      </c>
+      <c r="J13" s="9">
+        <v>0.61</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>17</v>
@@ -1560,24 +1578,24 @@
         <v>2020</v>
       </c>
       <c r="G14" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="H14" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I14">
         <v>1</v>
       </c>
       <c r="J14" s="8">
-        <v>0.06</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
         <v>11</v>
@@ -1589,27 +1607,27 @@
         <v>12</v>
       </c>
       <c r="F15">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="G15" t="s">
-        <v>27</v>
-      </c>
-      <c r="H15" t="s">
-        <v>28</v>
+        <v>13</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="I15">
-        <v>1</v>
-      </c>
-      <c r="J15" s="8">
-        <v>0.06</v>
+        <v>3</v>
+      </c>
+      <c r="J15" s="9">
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
         <v>11</v>
@@ -1621,27 +1639,27 @@
         <v>12</v>
       </c>
       <c r="F16">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="G16" t="s">
-        <v>27</v>
-      </c>
-      <c r="H16" t="s">
-        <v>28</v>
+        <v>13</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="I16">
-        <v>1</v>
-      </c>
-      <c r="J16" s="8">
-        <v>7.0000000000000007E-2</v>
+        <v>2</v>
+      </c>
+      <c r="J16" s="9">
+        <v>0.18</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C17" t="s">
         <v>11</v>
@@ -1653,27 +1671,27 @@
         <v>12</v>
       </c>
       <c r="F17">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="G17" t="s">
-        <v>27</v>
-      </c>
-      <c r="H17" t="s">
-        <v>28</v>
+        <v>13</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="I17">
         <v>1</v>
       </c>
-      <c r="J17" s="8">
-        <v>0.06</v>
+      <c r="J17" s="9">
+        <v>0.24</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C18" t="s">
         <v>11</v>
@@ -1688,24 +1706,24 @@
         <v>2020</v>
       </c>
       <c r="G18" t="s">
-        <v>27</v>
-      </c>
-      <c r="H18" t="s">
-        <v>28</v>
+        <v>13</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="I18">
-        <v>1</v>
-      </c>
-      <c r="J18" s="8">
-        <v>0.06</v>
+        <v>2</v>
+      </c>
+      <c r="J18" s="9">
+        <v>0.6</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
         <v>11</v>
@@ -1720,24 +1738,24 @@
         <v>2020</v>
       </c>
       <c r="G19" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="H19" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I19">
         <v>1</v>
       </c>
       <c r="J19" s="8">
-        <v>7.0000000000000007E-2</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C20" t="s">
         <v>11</v>
@@ -1749,27 +1767,27 @@
         <v>12</v>
       </c>
       <c r="F20">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="G20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H20" t="s">
-        <v>28</v>
+        <v>13</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="I20">
-        <v>1</v>
-      </c>
-      <c r="J20" s="8">
-        <v>0.08</v>
+        <v>3</v>
+      </c>
+      <c r="J20" s="9">
+        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C21" t="s">
         <v>11</v>
@@ -1781,27 +1799,27 @@
         <v>12</v>
       </c>
       <c r="F21">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="G21" t="s">
-        <v>27</v>
-      </c>
-      <c r="H21" t="s">
-        <v>28</v>
+        <v>13</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="I21">
-        <v>1</v>
-      </c>
-      <c r="J21" s="8">
-        <v>0.06</v>
+        <v>2</v>
+      </c>
+      <c r="J21" s="9">
+        <v>0.17</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C22" t="s">
         <v>11</v>
@@ -1813,27 +1831,27 @@
         <v>12</v>
       </c>
       <c r="F22">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="G22" t="s">
-        <v>27</v>
-      </c>
-      <c r="H22" t="s">
-        <v>28</v>
+        <v>13</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="I22">
         <v>1</v>
       </c>
-      <c r="J22" s="8">
-        <v>0.06</v>
+      <c r="J22" s="9">
+        <v>0.25</v>
       </c>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C23" t="s">
         <v>11</v>
@@ -1848,24 +1866,24 @@
         <v>2020</v>
       </c>
       <c r="G23" t="s">
-        <v>27</v>
-      </c>
-      <c r="H23" t="s">
-        <v>29</v>
+        <v>13</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="I23">
         <v>2</v>
       </c>
       <c r="J23" s="9">
-        <v>0.95</v>
+        <v>0.45999999999999996</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C24" t="s">
         <v>11</v>
@@ -1880,24 +1898,24 @@
         <v>2020</v>
       </c>
       <c r="G24" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="H24" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="I24">
-        <v>2</v>
-      </c>
-      <c r="J24" s="9">
-        <v>0.94</v>
+        <v>1</v>
+      </c>
+      <c r="J24" s="8">
+        <v>0.54</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C25" t="s">
         <v>11</v>
@@ -1909,24 +1927,24 @@
         <v>12</v>
       </c>
       <c r="F25">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="G25" t="s">
-        <v>27</v>
-      </c>
-      <c r="H25" t="s">
-        <v>29</v>
+        <v>13</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="I25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J25" s="9">
-        <v>0.94</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>20</v>
@@ -1941,27 +1959,27 @@
         <v>12</v>
       </c>
       <c r="F26">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="G26" t="s">
-        <v>27</v>
-      </c>
-      <c r="H26" t="s">
-        <v>29</v>
+        <v>13</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="I26">
         <v>2</v>
       </c>
       <c r="J26" s="9">
-        <v>0.92999999999999994</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C27" t="s">
         <v>11</v>
@@ -1973,27 +1991,27 @@
         <v>12</v>
       </c>
       <c r="F27">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="G27" t="s">
-        <v>27</v>
-      </c>
-      <c r="H27" t="s">
-        <v>29</v>
+        <v>13</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="I27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J27" s="9">
-        <v>0.94</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="28" spans="1:10">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C28" t="s">
         <v>11</v>
@@ -2008,24 +2026,24 @@
         <v>2020</v>
       </c>
       <c r="G28" t="s">
-        <v>27</v>
-      </c>
-      <c r="H28" t="s">
-        <v>29</v>
+        <v>13</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="I28">
         <v>2</v>
       </c>
       <c r="J28" s="9">
-        <v>0.94</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="29" spans="1:10">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C29" t="s">
         <v>11</v>
@@ -2040,24 +2058,24 @@
         <v>2020</v>
       </c>
       <c r="G29" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="H29" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="I29">
-        <v>2</v>
-      </c>
-      <c r="J29" s="9">
-        <v>0.92999999999999994</v>
+        <v>1</v>
+      </c>
+      <c r="J29" s="8">
+        <v>0.45</v>
       </c>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C30" t="s">
         <v>11</v>
@@ -2069,27 +2087,27 @@
         <v>12</v>
       </c>
       <c r="F30">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="G30" t="s">
-        <v>27</v>
-      </c>
-      <c r="H30" t="s">
-        <v>29</v>
+        <v>13</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="I30">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J30" s="9">
-        <v>0.92</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C31" t="s">
         <v>11</v>
@@ -2101,27 +2119,27 @@
         <v>12</v>
       </c>
       <c r="F31">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="G31" t="s">
-        <v>27</v>
-      </c>
-      <c r="H31" t="s">
-        <v>29</v>
+        <v>13</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="I31">
         <v>2</v>
       </c>
       <c r="J31" s="9">
-        <v>0.94</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C32" t="s">
         <v>11</v>
@@ -2133,19 +2151,19 @@
         <v>12</v>
       </c>
       <c r="F32">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="G32" t="s">
-        <v>27</v>
-      </c>
-      <c r="H32" t="s">
-        <v>29</v>
+        <v>13</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="I32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J32" s="9">
-        <v>0.94</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -2153,7 +2171,7 @@
         <v>10</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C33" t="s">
         <v>11</v>
@@ -2170,14 +2188,14 @@
       <c r="G33" t="s">
         <v>13</v>
       </c>
-      <c r="H33" t="s">
-        <v>25</v>
+      <c r="H33" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="I33">
-        <v>1</v>
-      </c>
-      <c r="J33" s="8">
-        <v>0.34</v>
+        <v>2</v>
+      </c>
+      <c r="J33" s="9">
+        <v>0.62</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -2185,7 +2203,7 @@
         <v>10</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C34" t="s">
         <v>11</v>
@@ -2209,7 +2227,7 @@
         <v>1</v>
       </c>
       <c r="J34" s="8">
-        <v>0.39</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -2217,7 +2235,7 @@
         <v>10</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C35" t="s">
         <v>11</v>
@@ -2229,19 +2247,19 @@
         <v>12</v>
       </c>
       <c r="F35">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="G35" t="s">
         <v>13</v>
       </c>
-      <c r="H35" t="s">
-        <v>25</v>
+      <c r="H35" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="I35">
-        <v>1</v>
-      </c>
-      <c r="J35" s="8">
-        <v>0.4</v>
+        <v>3</v>
+      </c>
+      <c r="J35" s="9">
+        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -2249,7 +2267,7 @@
         <v>10</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C36" t="s">
         <v>11</v>
@@ -2261,19 +2279,19 @@
         <v>12</v>
       </c>
       <c r="F36">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="G36" t="s">
         <v>13</v>
       </c>
-      <c r="H36" t="s">
-        <v>25</v>
+      <c r="H36" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="I36">
-        <v>1</v>
-      </c>
-      <c r="J36" s="8">
-        <v>0.54</v>
+        <v>2</v>
+      </c>
+      <c r="J36" s="9">
+        <v>0.18</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -2281,7 +2299,7 @@
         <v>10</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C37" t="s">
         <v>11</v>
@@ -2293,19 +2311,19 @@
         <v>12</v>
       </c>
       <c r="F37">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="G37" t="s">
         <v>13</v>
       </c>
-      <c r="H37" t="s">
-        <v>25</v>
+      <c r="H37" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="I37">
         <v>1</v>
       </c>
-      <c r="J37" s="8">
-        <v>0.45</v>
+      <c r="J37" s="9">
+        <v>0.24</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -2313,7 +2331,7 @@
         <v>10</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C38" t="s">
         <v>11</v>
@@ -2330,14 +2348,14 @@
       <c r="G38" t="s">
         <v>13</v>
       </c>
-      <c r="H38" t="s">
-        <v>25</v>
+      <c r="H38" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="I38">
-        <v>1</v>
-      </c>
-      <c r="J38" s="8">
-        <v>0.38</v>
+        <v>2</v>
+      </c>
+      <c r="J38" s="9">
+        <v>0.6</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -2377,7 +2395,7 @@
         <v>10</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C40" t="s">
         <v>11</v>
@@ -2389,19 +2407,19 @@
         <v>12</v>
       </c>
       <c r="F40">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="G40" t="s">
         <v>13</v>
       </c>
-      <c r="H40" t="s">
-        <v>25</v>
+      <c r="H40" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="I40">
-        <v>1</v>
-      </c>
-      <c r="J40" s="8">
-        <v>0.42</v>
+        <v>3</v>
+      </c>
+      <c r="J40" s="9">
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -2409,7 +2427,7 @@
         <v>10</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C41" t="s">
         <v>11</v>
@@ -2421,19 +2439,19 @@
         <v>12</v>
       </c>
       <c r="F41">
-        <v>2016</v>
+        <v>2022</v>
       </c>
       <c r="G41" t="s">
         <v>13</v>
       </c>
-      <c r="H41" t="s">
-        <v>25</v>
+      <c r="H41" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="I41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J41" s="9">
-        <v>0.44</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -2441,7 +2459,7 @@
         <v>10</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C42" t="s">
         <v>11</v>
@@ -2453,19 +2471,19 @@
         <v>12</v>
       </c>
       <c r="F42">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="G42" t="s">
         <v>13</v>
       </c>
-      <c r="H42" t="s">
-        <v>25</v>
+      <c r="H42" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="I42">
         <v>1</v>
       </c>
-      <c r="J42" s="8">
-        <v>0.39</v>
+      <c r="J42" s="9">
+        <v>0.24</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -2473,7 +2491,7 @@
         <v>10</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C43" t="s">
         <v>11</v>
@@ -2490,14 +2508,14 @@
       <c r="G43" t="s">
         <v>13</v>
       </c>
-      <c r="H43" t="s">
-        <v>25</v>
+      <c r="H43" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="I43">
-        <v>1</v>
-      </c>
-      <c r="J43" s="8">
-        <v>0.27</v>
+        <v>2</v>
+      </c>
+      <c r="J43" s="9">
+        <v>0.58000000000000007</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -2505,7 +2523,7 @@
         <v>10</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C44" t="s">
         <v>11</v>
@@ -2517,19 +2535,19 @@
         <v>12</v>
       </c>
       <c r="F44">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="G44" t="s">
         <v>13</v>
       </c>
-      <c r="H44" s="6" t="s">
-        <v>32</v>
+      <c r="H44" t="s">
+        <v>25</v>
       </c>
       <c r="I44">
-        <v>2</v>
-      </c>
-      <c r="J44" s="9">
-        <v>0.18</v>
+        <v>1</v>
+      </c>
+      <c r="J44" s="8">
+        <v>0.42</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -2537,7 +2555,7 @@
         <v>10</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C45" t="s">
         <v>11</v>
@@ -2555,13 +2573,13 @@
         <v>13</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I45">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J45" s="9">
-        <v>0.18</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -2569,7 +2587,7 @@
         <v>10</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C46" t="s">
         <v>11</v>
@@ -2593,7 +2611,7 @@
         <v>2</v>
       </c>
       <c r="J46" s="9">
-        <v>0.17</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -2601,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C47" t="s">
         <v>11</v>
@@ -2618,14 +2636,14 @@
       <c r="G47" t="s">
         <v>13</v>
       </c>
-      <c r="H47" s="6" t="s">
-        <v>32</v>
+      <c r="H47" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="I47">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J47" s="9">
-        <v>0.24</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -2633,7 +2651,7 @@
         <v>10</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C48" t="s">
         <v>11</v>
@@ -2645,19 +2663,19 @@
         <v>12</v>
       </c>
       <c r="F48">
-        <v>2022</v>
+        <v>2016</v>
       </c>
       <c r="G48" t="s">
         <v>13</v>
       </c>
       <c r="H48" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I48">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J48" s="9">
-        <v>0.2</v>
+        <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -2665,7 +2683,7 @@
         <v>10</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C49" t="s">
         <v>11</v>
@@ -2677,19 +2695,19 @@
         <v>12</v>
       </c>
       <c r="F49">
-        <v>2022</v>
+        <v>2016</v>
       </c>
       <c r="G49" t="s">
         <v>13</v>
       </c>
-      <c r="H49" s="6" t="s">
-        <v>32</v>
+      <c r="H49" t="s">
+        <v>25</v>
       </c>
       <c r="I49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J49" s="9">
-        <v>0.18</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -2697,7 +2715,7 @@
         <v>10</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C50" t="s">
         <v>11</v>
@@ -2709,19 +2727,19 @@
         <v>12</v>
       </c>
       <c r="F50">
-        <v>2022</v>
+        <v>2018</v>
       </c>
       <c r="G50" t="s">
         <v>13</v>
       </c>
       <c r="H50" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I50">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J50" s="9">
-        <v>0.19</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -2729,7 +2747,7 @@
         <v>10</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C51" t="s">
         <v>11</v>
@@ -2741,7 +2759,7 @@
         <v>12</v>
       </c>
       <c r="F51">
-        <v>2022</v>
+        <v>2018</v>
       </c>
       <c r="G51" t="s">
         <v>13</v>
@@ -2753,7 +2771,7 @@
         <v>2</v>
       </c>
       <c r="J51" s="9">
-        <v>0.19</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -2778,14 +2796,14 @@
       <c r="G52" t="s">
         <v>13</v>
       </c>
-      <c r="H52" s="6" t="s">
-        <v>32</v>
+      <c r="H52" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="I52">
-        <v>2</v>
-      </c>
-      <c r="J52" s="9">
-        <v>0.2</v>
+        <v>1</v>
+      </c>
+      <c r="J52" s="8">
+        <v>0.27</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -2805,19 +2823,19 @@
         <v>12</v>
       </c>
       <c r="F53">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="G53" t="s">
         <v>13</v>
       </c>
       <c r="H53" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I53">
         <v>2</v>
       </c>
       <c r="J53" s="9">
-        <v>0.18</v>
+        <v>0.61</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -2825,7 +2843,7 @@
         <v>10</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C54" t="s">
         <v>11</v>
@@ -2837,19 +2855,19 @@
         <v>12</v>
       </c>
       <c r="F54">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="G54" t="s">
         <v>13</v>
       </c>
-      <c r="H54" s="6" t="s">
-        <v>32</v>
+      <c r="H54" t="s">
+        <v>25</v>
       </c>
       <c r="I54">
-        <v>2</v>
-      </c>
-      <c r="J54" s="9">
-        <v>0.15</v>
+        <v>1</v>
+      </c>
+      <c r="J54" s="8">
+        <v>0.39</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -2857,7 +2875,7 @@
         <v>10</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C55" t="s">
         <v>11</v>
@@ -2869,7 +2887,7 @@
         <v>12</v>
       </c>
       <c r="F55">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="G55" t="s">
         <v>13</v>
@@ -2878,10 +2896,10 @@
         <v>31</v>
       </c>
       <c r="I55">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J55" s="9">
-        <v>0.65999999999999992</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -2889,7 +2907,7 @@
         <v>10</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C56" t="s">
         <v>11</v>
@@ -2901,19 +2919,19 @@
         <v>12</v>
       </c>
       <c r="F56">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="G56" t="s">
         <v>13</v>
       </c>
       <c r="H56" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I56">
         <v>2</v>
       </c>
       <c r="J56" s="9">
-        <v>0.61</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -2921,7 +2939,7 @@
         <v>10</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C57" t="s">
         <v>11</v>
@@ -2933,19 +2951,19 @@
         <v>12</v>
       </c>
       <c r="F57">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="G57" t="s">
         <v>13</v>
       </c>
-      <c r="H57" s="6" t="s">
-        <v>31</v>
+      <c r="H57" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="I57">
-        <v>2</v>
-      </c>
-      <c r="J57" s="9">
-        <v>0.6</v>
+        <v>1</v>
+      </c>
+      <c r="J57" s="8">
+        <v>0.25</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -2953,7 +2971,7 @@
         <v>10</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C58" t="s">
         <v>11</v>
@@ -2977,7 +2995,7 @@
         <v>2</v>
       </c>
       <c r="J58" s="9">
-        <v>0.45999999999999996</v>
+        <v>0.73</v>
       </c>
     </row>
     <row r="59" spans="1:10">
@@ -2985,7 +3003,7 @@
         <v>10</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C59" t="s">
         <v>11</v>
@@ -3002,14 +3020,14 @@
       <c r="G59" t="s">
         <v>13</v>
       </c>
-      <c r="H59" s="6" t="s">
-        <v>31</v>
+      <c r="H59" t="s">
+        <v>25</v>
       </c>
       <c r="I59">
-        <v>2</v>
-      </c>
-      <c r="J59" s="9">
-        <v>0.55000000000000004</v>
+        <v>1</v>
+      </c>
+      <c r="J59" s="8">
+        <v>0.27</v>
       </c>
     </row>
     <row r="60" spans="1:10">
@@ -3017,7 +3035,7 @@
         <v>10</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C60" t="s">
         <v>11</v>
@@ -3029,7 +3047,7 @@
         <v>12</v>
       </c>
       <c r="F60">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="G60" t="s">
         <v>13</v>
@@ -3038,10 +3056,10 @@
         <v>31</v>
       </c>
       <c r="I60">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J60" s="9">
-        <v>0.62</v>
+        <v>0.64</v>
       </c>
     </row>
     <row r="61" spans="1:10">
@@ -3049,7 +3067,7 @@
         <v>10</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C61" t="s">
         <v>11</v>
@@ -3061,19 +3079,19 @@
         <v>12</v>
       </c>
       <c r="F61">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="G61" t="s">
         <v>13</v>
       </c>
       <c r="H61" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I61">
         <v>2</v>
       </c>
       <c r="J61" s="9">
-        <v>0.6</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="62" spans="1:10">
@@ -3081,7 +3099,7 @@
         <v>10</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C62" t="s">
         <v>11</v>
@@ -3093,27 +3111,27 @@
         <v>12</v>
       </c>
       <c r="F62">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="G62" t="s">
         <v>13</v>
       </c>
-      <c r="H62" s="6" t="s">
-        <v>31</v>
+      <c r="H62" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="I62">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J62" s="9">
-        <v>0.58000000000000007</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="63" spans="1:10">
       <c r="A63" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C63" t="s">
         <v>11</v>
@@ -3125,27 +3143,27 @@
         <v>12</v>
       </c>
       <c r="F63">
-        <v>2016</v>
+        <v>2020</v>
       </c>
       <c r="G63" t="s">
-        <v>13</v>
-      </c>
-      <c r="H63" s="6" t="s">
-        <v>31</v>
+        <v>27</v>
+      </c>
+      <c r="H63" t="s">
+        <v>28</v>
       </c>
       <c r="I63">
-        <v>3</v>
-      </c>
-      <c r="J63" s="9">
-        <v>0.56000000000000005</v>
+        <v>1</v>
+      </c>
+      <c r="J63" s="8">
+        <v>0.05</v>
       </c>
     </row>
     <row r="64" spans="1:10">
       <c r="A64" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C64" t="s">
         <v>11</v>
@@ -3160,24 +3178,24 @@
         <v>2020</v>
       </c>
       <c r="G64" t="s">
-        <v>13</v>
-      </c>
-      <c r="H64" s="6" t="s">
-        <v>31</v>
+        <v>27</v>
+      </c>
+      <c r="H64" t="s">
+        <v>29</v>
       </c>
       <c r="I64">
         <v>2</v>
       </c>
       <c r="J64" s="9">
-        <v>0.61</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10">
       <c r="A65" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C65" t="s">
         <v>11</v>
@@ -3192,56 +3210,56 @@
         <v>2020</v>
       </c>
       <c r="G65" t="s">
-        <v>13</v>
-      </c>
-      <c r="H65" s="6" t="s">
-        <v>31</v>
+        <v>27</v>
+      </c>
+      <c r="H65" t="s">
+        <v>28</v>
       </c>
       <c r="I65">
+        <v>1</v>
+      </c>
+      <c r="J65" s="8">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10">
+      <c r="A66" t="s">
+        <v>26</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C66" t="s">
+        <v>11</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F66">
+        <v>2020</v>
+      </c>
+      <c r="G66" t="s">
+        <v>27</v>
+      </c>
+      <c r="H66" t="s">
+        <v>29</v>
+      </c>
+      <c r="I66">
         <v>2</v>
       </c>
-      <c r="J65" s="9">
-        <v>0.73</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11">
-      <c r="A66" t="s">
-        <v>10</v>
-      </c>
-      <c r="B66" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C66" t="s">
-        <v>11</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E66" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F66">
-        <v>2022</v>
-      </c>
-      <c r="G66" t="s">
-        <v>13</v>
-      </c>
-      <c r="H66" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I66">
-        <v>1</v>
-      </c>
-      <c r="J66" s="8">
-        <v>0.24</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11">
+      <c r="J66" s="9">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10">
       <c r="A67" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C67" t="s">
         <v>11</v>
@@ -3253,24 +3271,24 @@
         <v>12</v>
       </c>
       <c r="F67">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="G67" t="s">
-        <v>13</v>
-      </c>
-      <c r="H67" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
+      </c>
+      <c r="H67" t="s">
+        <v>28</v>
       </c>
       <c r="I67">
         <v>1</v>
       </c>
-      <c r="J67" s="9">
-        <v>0.24</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11">
+      <c r="J67" s="8">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10">
       <c r="A68" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="B68" s="7" t="s">
         <v>18</v>
@@ -3285,24 +3303,24 @@
         <v>12</v>
       </c>
       <c r="F68">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="G68" t="s">
-        <v>13</v>
-      </c>
-      <c r="H68" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
+      </c>
+      <c r="H68" t="s">
+        <v>29</v>
       </c>
       <c r="I68">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J68" s="9">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10">
       <c r="A69" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="B69" s="7" t="s">
         <v>20</v>
@@ -3317,60 +3335,60 @@
         <v>12</v>
       </c>
       <c r="F69">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="G69" t="s">
-        <v>13</v>
-      </c>
-      <c r="H69" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
+      </c>
+      <c r="H69" t="s">
+        <v>28</v>
       </c>
       <c r="I69">
         <v>1</v>
       </c>
-      <c r="J69" s="9">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11">
+      <c r="J69" s="8">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10">
       <c r="A70" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="B70" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C70" t="s">
+        <v>11</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F70">
+        <v>2020</v>
+      </c>
+      <c r="G70" t="s">
+        <v>27</v>
+      </c>
+      <c r="H70" t="s">
+        <v>29</v>
+      </c>
+      <c r="I70">
+        <v>2</v>
+      </c>
+      <c r="J70" s="9">
+        <v>0.92999999999999994</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10">
+      <c r="A71" t="s">
+        <v>26</v>
+      </c>
+      <c r="B71" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C70" t="s">
-        <v>11</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E70" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F70">
-        <v>2022</v>
-      </c>
-      <c r="G70" t="s">
-        <v>13</v>
-      </c>
-      <c r="H70" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I70">
-        <v>1</v>
-      </c>
-      <c r="J70" s="9">
-        <v>0.32</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11">
-      <c r="A71" t="s">
-        <v>10</v>
-      </c>
-      <c r="B71" s="7" t="s">
-        <v>22</v>
-      </c>
       <c r="C71" t="s">
         <v>11</v>
       </c>
@@ -3381,27 +3399,27 @@
         <v>12</v>
       </c>
       <c r="F71">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="G71" t="s">
-        <v>13</v>
-      </c>
-      <c r="H71" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
+      </c>
+      <c r="H71" t="s">
+        <v>28</v>
       </c>
       <c r="I71">
         <v>1</v>
       </c>
-      <c r="J71" s="9">
-        <v>0.24</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11">
+      <c r="J71" s="8">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10">
       <c r="A72" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C72" t="s">
         <v>11</v>
@@ -3413,27 +3431,27 @@
         <v>12</v>
       </c>
       <c r="F72">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="G72" t="s">
-        <v>13</v>
-      </c>
-      <c r="H72" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
+      </c>
+      <c r="H72" t="s">
+        <v>29</v>
       </c>
       <c r="I72">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J72" s="9">
-        <v>0.24</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10">
       <c r="A73" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C73" t="s">
         <v>11</v>
@@ -3445,27 +3463,27 @@
         <v>12</v>
       </c>
       <c r="F73">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="G73" t="s">
-        <v>13</v>
-      </c>
-      <c r="H73" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
+      </c>
+      <c r="H73" t="s">
+        <v>28</v>
       </c>
       <c r="I73">
         <v>1</v>
       </c>
-      <c r="J73" s="9">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11">
+      <c r="J73" s="8">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10">
       <c r="A74" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C74" t="s">
         <v>11</v>
@@ -3477,27 +3495,27 @@
         <v>12</v>
       </c>
       <c r="F74">
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="G74" t="s">
-        <v>13</v>
-      </c>
-      <c r="H74" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
+      </c>
+      <c r="H74" t="s">
+        <v>29</v>
       </c>
       <c r="I74">
-        <v>1</v>
-      </c>
-      <c r="J74" s="8">
-        <v>0.27</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11">
+        <v>2</v>
+      </c>
+      <c r="J74" s="9">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10">
       <c r="A75" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C75" t="s">
         <v>11</v>
@@ -3509,27 +3527,27 @@
         <v>12</v>
       </c>
       <c r="F75">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="G75" t="s">
-        <v>13</v>
-      </c>
-      <c r="H75" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
+      </c>
+      <c r="H75" t="s">
+        <v>28</v>
       </c>
       <c r="I75">
         <v>1</v>
       </c>
       <c r="J75" s="8">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10">
       <c r="A76" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C76" t="s">
         <v>11</v>
@@ -3541,229 +3559,211 @@
         <v>12</v>
       </c>
       <c r="F76">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="G76" t="s">
-        <v>13</v>
-      </c>
-      <c r="H76" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
+      </c>
+      <c r="H76" t="s">
+        <v>29</v>
       </c>
       <c r="I76">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J76" s="9">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11">
+        <v>0.92999999999999994</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10">
       <c r="A77" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C77" t="s">
         <v>11</v>
       </c>
-      <c r="D77" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E77" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F77" s="10">
-        <v>2022</v>
+      <c r="D77" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F77">
+        <v>2020</v>
       </c>
       <c r="G77" t="s">
-        <v>34</v>
-      </c>
-      <c r="H77" s="6" t="s">
-        <v>35</v>
+        <v>27</v>
+      </c>
+      <c r="H77" t="s">
+        <v>28</v>
       </c>
       <c r="I77">
         <v>1</v>
       </c>
-      <c r="J77" s="9">
-        <v>0.15</v>
-      </c>
-      <c r="K77">
-        <v>1280</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11">
+      <c r="J77" s="8">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10">
       <c r="A78" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C78" t="s">
         <v>11</v>
       </c>
-      <c r="D78" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E78" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F78" s="10">
-        <v>2022</v>
+      <c r="D78" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E78" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F78">
+        <v>2020</v>
       </c>
       <c r="G78" t="s">
-        <v>34</v>
-      </c>
-      <c r="H78" s="6" t="s">
-        <v>36</v>
+        <v>27</v>
+      </c>
+      <c r="H78" t="s">
+        <v>29</v>
       </c>
       <c r="I78">
         <v>2</v>
       </c>
       <c r="J78" s="9">
-        <v>0.13</v>
-      </c>
-      <c r="K78">
-        <v>1141</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10">
       <c r="A79" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C79" t="s">
         <v>11</v>
       </c>
-      <c r="D79" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E79" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F79" s="10">
-        <v>2022</v>
+      <c r="D79" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F79">
+        <v>2020</v>
       </c>
       <c r="G79" t="s">
-        <v>34</v>
-      </c>
-      <c r="H79" s="6" t="s">
-        <v>37</v>
+        <v>27</v>
+      </c>
+      <c r="H79" t="s">
+        <v>28</v>
       </c>
       <c r="I79">
-        <v>3</v>
-      </c>
-      <c r="J79" s="9">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="K79">
-        <v>1181</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11">
+        <v>1</v>
+      </c>
+      <c r="J79" s="8">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10">
       <c r="A80" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C80" t="s">
         <v>11</v>
       </c>
-      <c r="D80" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E80" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F80" s="10">
-        <v>2022</v>
+      <c r="D80" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F80">
+        <v>2020</v>
       </c>
       <c r="G80" t="s">
-        <v>34</v>
-      </c>
-      <c r="H80" s="6" t="s">
-        <v>38</v>
+        <v>27</v>
+      </c>
+      <c r="H80" t="s">
+        <v>29</v>
       </c>
       <c r="I80">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J80" s="9">
-        <v>0.22</v>
-      </c>
-      <c r="K80">
-        <v>1891</v>
+        <v>0.94</v>
       </c>
     </row>
     <row r="81" spans="1:11">
       <c r="A81" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C81" t="s">
         <v>11</v>
       </c>
-      <c r="D81" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E81" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F81" s="10">
-        <v>2022</v>
+      <c r="D81" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F81">
+        <v>2020</v>
       </c>
       <c r="G81" t="s">
-        <v>34</v>
-      </c>
-      <c r="H81" s="6" t="s">
-        <v>39</v>
+        <v>27</v>
+      </c>
+      <c r="H81" t="s">
+        <v>28</v>
       </c>
       <c r="I81">
-        <v>5</v>
-      </c>
-      <c r="J81" s="9">
-        <v>0.17</v>
-      </c>
-      <c r="K81">
-        <v>1480</v>
+        <v>1</v>
+      </c>
+      <c r="J81" s="8">
+        <v>0.06</v>
       </c>
     </row>
     <row r="82" spans="1:11">
       <c r="A82" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C82" t="s">
         <v>11</v>
       </c>
-      <c r="D82" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E82" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F82" s="10">
-        <v>2022</v>
+      <c r="D82" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F82">
+        <v>2020</v>
       </c>
       <c r="G82" t="s">
-        <v>34</v>
-      </c>
-      <c r="H82" s="6" t="s">
-        <v>40</v>
+        <v>27</v>
+      </c>
+      <c r="H82" t="s">
+        <v>29</v>
       </c>
       <c r="I82">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="J82" s="9">
-        <v>0.18</v>
-      </c>
-      <c r="K82">
-        <v>1544</v>
+        <v>0.94</v>
       </c>
     </row>
     <row r="83" spans="1:11">
@@ -3783,27 +3783,24 @@
         <v>12</v>
       </c>
       <c r="F83" s="10">
-        <v>2022</v>
+        <v>2016</v>
       </c>
       <c r="G83" t="s">
         <v>34</v>
       </c>
       <c r="H83" s="6" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="I83">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="J83" s="9">
-        <v>0.16</v>
-      </c>
-      <c r="K83">
-        <v>8779</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="84" spans="1:11">
       <c r="A84" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B84" s="7" t="s">
         <v>42</v>
@@ -3818,22 +3815,19 @@
         <v>12</v>
       </c>
       <c r="F84" s="10">
-        <v>2022</v>
+        <v>2016</v>
       </c>
       <c r="G84" t="s">
         <v>34</v>
       </c>
       <c r="H84" s="6" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="I84">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J84" s="9">
-        <v>0.19</v>
-      </c>
-      <c r="K84">
-        <v>10289</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="85" spans="1:11">
@@ -3853,27 +3847,24 @@
         <v>12</v>
       </c>
       <c r="F85" s="10">
-        <v>2022</v>
+        <v>2016</v>
       </c>
       <c r="G85" t="s">
         <v>34</v>
       </c>
       <c r="H85" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I85">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J85" s="9">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="K85">
-        <v>7522</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="86" spans="1:11">
       <c r="A86" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B86" s="7" t="s">
         <v>42</v>
@@ -3888,22 +3879,19 @@
         <v>12</v>
       </c>
       <c r="F86" s="10">
-        <v>2022</v>
+        <v>2016</v>
       </c>
       <c r="G86" t="s">
         <v>34</v>
       </c>
       <c r="H86" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I86">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J86" s="9">
-        <v>0.15</v>
-      </c>
-      <c r="K86">
-        <v>8330</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="87" spans="1:11">
@@ -3923,27 +3911,24 @@
         <v>12</v>
       </c>
       <c r="F87" s="10">
-        <v>2022</v>
+        <v>2016</v>
       </c>
       <c r="G87" t="s">
         <v>34</v>
       </c>
       <c r="H87" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I87">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J87" s="9">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="K87">
-        <v>7770</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="88" spans="1:11">
       <c r="A88" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B88" s="7" t="s">
         <v>42</v>
@@ -3958,22 +3943,19 @@
         <v>12</v>
       </c>
       <c r="F88" s="10">
-        <v>2022</v>
+        <v>2016</v>
       </c>
       <c r="G88" t="s">
         <v>34</v>
       </c>
       <c r="H88" s="6" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="I88">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="J88" s="9">
-        <v>0.15</v>
-      </c>
-      <c r="K88">
-        <v>8073</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="89" spans="1:11">
@@ -3993,27 +3975,24 @@
         <v>12</v>
       </c>
       <c r="F89" s="10">
-        <v>2022</v>
+        <v>2018</v>
       </c>
       <c r="G89" t="s">
         <v>34</v>
       </c>
       <c r="H89" s="6" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="I89">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="J89" s="9">
-        <v>0.22</v>
-      </c>
-      <c r="K89">
-        <v>11771</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="90" spans="1:11">
       <c r="A90" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B90" s="7" t="s">
         <v>42</v>
@@ -4028,22 +4007,19 @@
         <v>12</v>
       </c>
       <c r="F90" s="10">
-        <v>2022</v>
+        <v>2018</v>
       </c>
       <c r="G90" t="s">
         <v>34</v>
       </c>
       <c r="H90" s="6" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="I90">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J90" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="K90">
-        <v>11043</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="91" spans="1:11">
@@ -4063,27 +4039,24 @@
         <v>12</v>
       </c>
       <c r="F91" s="10">
-        <v>2022</v>
+        <v>2018</v>
       </c>
       <c r="G91" t="s">
         <v>34</v>
       </c>
       <c r="H91" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I91">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J91" s="9">
-        <v>0.17</v>
-      </c>
-      <c r="K91">
-        <v>9030</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="92" spans="1:11">
       <c r="A92" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B92" s="7" t="s">
         <v>42</v>
@@ -4098,22 +4071,19 @@
         <v>12</v>
       </c>
       <c r="F92" s="10">
-        <v>2022</v>
+        <v>2018</v>
       </c>
       <c r="G92" t="s">
         <v>34</v>
       </c>
       <c r="H92" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I92">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J92" s="9">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="K92">
-        <v>7830</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="93" spans="1:11">
@@ -4133,27 +4103,24 @@
         <v>12</v>
       </c>
       <c r="F93" s="10">
-        <v>2022</v>
+        <v>2018</v>
       </c>
       <c r="G93" t="s">
         <v>34</v>
       </c>
       <c r="H93" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I93">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J93" s="9">
-        <v>0.17</v>
-      </c>
-      <c r="K93">
-        <v>9507</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="94" spans="1:11">
       <c r="A94" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B94" s="7" t="s">
         <v>42</v>
@@ -4168,22 +4135,19 @@
         <v>12</v>
       </c>
       <c r="F94" s="10">
-        <v>2022</v>
+        <v>2018</v>
       </c>
       <c r="G94" t="s">
         <v>34</v>
       </c>
       <c r="H94" s="6" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="I94">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="J94" s="9">
-        <v>0.16</v>
-      </c>
-      <c r="K94">
-        <v>8960</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="95" spans="1:11">
@@ -4244,16 +4208,16 @@
         <v>34</v>
       </c>
       <c r="H96" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I96">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J96" s="9">
-        <v>0.13</v>
-      </c>
-    </row>
-    <row r="97" spans="1:10">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11">
       <c r="A97" t="s">
         <v>33</v>
       </c>
@@ -4276,16 +4240,16 @@
         <v>34</v>
       </c>
       <c r="H97" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I97">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J97" s="9">
-        <v>0.18</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11">
       <c r="A98" t="s">
         <v>33</v>
       </c>
@@ -4308,16 +4272,16 @@
         <v>34</v>
       </c>
       <c r="H98" s="6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="I98">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J98" s="9">
-        <v>0.14000000000000001</v>
-      </c>
-    </row>
-    <row r="99" spans="1:10">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11">
       <c r="A99" t="s">
         <v>33</v>
       </c>
@@ -4340,16 +4304,16 @@
         <v>34</v>
       </c>
       <c r="H99" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I99">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J99" s="9">
-        <v>0.17</v>
-      </c>
-    </row>
-    <row r="100" spans="1:10">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11">
       <c r="A100" t="s">
         <v>33</v>
       </c>
@@ -4381,12 +4345,12 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="101" spans="1:10">
+    <row r="101" spans="1:11">
       <c r="A101" t="s">
         <v>33</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="C101" t="s">
         <v>11</v>
@@ -4398,27 +4362,30 @@
         <v>12</v>
       </c>
       <c r="F101" s="10">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="G101" t="s">
         <v>34</v>
       </c>
       <c r="H101" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I101">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J101" s="9">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="K101">
+        <v>7770</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11">
       <c r="A102" t="s">
         <v>33</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="C102" t="s">
         <v>11</v>
@@ -4430,7 +4397,7 @@
         <v>12</v>
       </c>
       <c r="F102" s="10">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="G102" t="s">
         <v>34</v>
@@ -4442,15 +4409,18 @@
         <v>5</v>
       </c>
       <c r="J102" s="9">
-        <v>0.13</v>
-      </c>
-    </row>
-    <row r="103" spans="1:10">
+        <v>0.17</v>
+      </c>
+      <c r="K102">
+        <v>9507</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11">
       <c r="A103" t="s">
         <v>33</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="C103" t="s">
         <v>11</v>
@@ -4462,27 +4432,30 @@
         <v>12</v>
       </c>
       <c r="F103" s="10">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="G103" t="s">
         <v>34</v>
       </c>
       <c r="H103" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I103">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J103" s="9">
-        <v>0.18</v>
-      </c>
-    </row>
-    <row r="104" spans="1:10">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="K103">
+        <v>7522</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11">
       <c r="A104" t="s">
         <v>33</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="C104" t="s">
         <v>11</v>
@@ -4494,7 +4467,7 @@
         <v>12</v>
       </c>
       <c r="F104" s="10">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="G104" t="s">
         <v>34</v>
@@ -4506,15 +4479,18 @@
         <v>3</v>
       </c>
       <c r="J104" s="9">
-        <v>0.14000000000000001</v>
-      </c>
-    </row>
-    <row r="105" spans="1:10">
+        <v>0.17</v>
+      </c>
+      <c r="K104">
+        <v>9030</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11">
       <c r="A105" t="s">
         <v>33</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="C105" t="s">
         <v>11</v>
@@ -4526,27 +4502,30 @@
         <v>12</v>
       </c>
       <c r="F105" s="10">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="G105" t="s">
         <v>34</v>
       </c>
       <c r="H105" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I105">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J105" s="9">
-        <v>0.17</v>
-      </c>
-    </row>
-    <row r="106" spans="1:10">
+        <v>0.16</v>
+      </c>
+      <c r="K105">
+        <v>8779</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11">
       <c r="A106" t="s">
         <v>33</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="C106" t="s">
         <v>11</v>
@@ -4558,7 +4537,7 @@
         <v>12</v>
       </c>
       <c r="F106" s="10">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="G106" t="s">
         <v>34</v>
@@ -4570,15 +4549,18 @@
         <v>1</v>
       </c>
       <c r="J106" s="9">
-        <v>0.26</v>
-      </c>
-    </row>
-    <row r="107" spans="1:10">
+        <v>0.22</v>
+      </c>
+      <c r="K106">
+        <v>11771</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11">
       <c r="A107" t="s">
         <v>33</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="C107" t="s">
         <v>11</v>
@@ -4590,7 +4572,7 @@
         <v>12</v>
       </c>
       <c r="F107" s="10">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="G107" t="s">
         <v>34</v>
@@ -4605,12 +4587,12 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="108" spans="1:10">
+    <row r="108" spans="1:11">
       <c r="A108" t="s">
         <v>33</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="C108" t="s">
         <v>11</v>
@@ -4622,27 +4604,27 @@
         <v>12</v>
       </c>
       <c r="F108" s="10">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="G108" t="s">
         <v>34</v>
       </c>
       <c r="H108" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="I108">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J108" s="9">
-        <v>0.13</v>
-      </c>
-    </row>
-    <row r="109" spans="1:10">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11">
       <c r="A109" t="s">
         <v>33</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="C109" t="s">
         <v>11</v>
@@ -4654,7 +4636,7 @@
         <v>12</v>
       </c>
       <c r="F109" s="10">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="G109" t="s">
         <v>34</v>
@@ -4666,15 +4648,15 @@
         <v>4</v>
       </c>
       <c r="J109" s="9">
-        <v>0.19</v>
-      </c>
-    </row>
-    <row r="110" spans="1:10">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11">
       <c r="A110" t="s">
         <v>33</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="C110" t="s">
         <v>11</v>
@@ -4686,27 +4668,27 @@
         <v>12</v>
       </c>
       <c r="F110" s="10">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="G110" t="s">
         <v>34</v>
       </c>
       <c r="H110" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I110">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J110" s="9">
         <v>0.15</v>
       </c>
     </row>
-    <row r="111" spans="1:10">
+    <row r="111" spans="1:11">
       <c r="A111" t="s">
         <v>33</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="C111" t="s">
         <v>11</v>
@@ -4718,27 +4700,27 @@
         <v>12</v>
       </c>
       <c r="F111" s="10">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="G111" t="s">
         <v>34</v>
       </c>
       <c r="H111" s="6" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="I111">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J111" s="9">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="112" spans="1:10">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11">
       <c r="A112" t="s">
         <v>33</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="C112" t="s">
         <v>11</v>
@@ -4750,22 +4732,22 @@
         <v>12</v>
       </c>
       <c r="F112" s="10">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="G112" t="s">
         <v>34</v>
       </c>
       <c r="H112" s="6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="I112">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J112" s="9">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="113" spans="1:10">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11">
       <c r="A113" t="s">
         <v>33</v>
       </c>
@@ -4797,7 +4779,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="114" spans="1:10">
+    <row r="114" spans="1:11">
       <c r="A114" t="s">
         <v>33</v>
       </c>
@@ -4820,16 +4802,16 @@
         <v>34</v>
       </c>
       <c r="H114" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="I114">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J114" s="9">
-        <v>0.14000000000000001</v>
-      </c>
-    </row>
-    <row r="115" spans="1:10">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11">
       <c r="A115" t="s">
         <v>33</v>
       </c>
@@ -4861,7 +4843,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="116" spans="1:10">
+    <row r="116" spans="1:11">
       <c r="A116" t="s">
         <v>33</v>
       </c>
@@ -4884,16 +4866,16 @@
         <v>34</v>
       </c>
       <c r="H116" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I116">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J116" s="9">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="117" spans="1:10">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11">
       <c r="A117" t="s">
         <v>33</v>
       </c>
@@ -4916,16 +4898,16 @@
         <v>34</v>
       </c>
       <c r="H117" s="6" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="I117">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J117" s="9">
-        <v>0.16</v>
-      </c>
-    </row>
-    <row r="118" spans="1:10">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11">
       <c r="A118" t="s">
         <v>33</v>
       </c>
@@ -4948,21 +4930,21 @@
         <v>34</v>
       </c>
       <c r="H118" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I118">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J118" s="9">
-        <v>0.24</v>
-      </c>
-    </row>
-    <row r="119" spans="1:10">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11">
       <c r="A119" t="s">
         <v>33</v>
       </c>
       <c r="B119" s="7" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="C119" t="s">
         <v>11</v>
@@ -4974,7 +4956,7 @@
         <v>12</v>
       </c>
       <c r="F119" s="10">
-        <v>2016</v>
+        <v>2020</v>
       </c>
       <c r="G119" t="s">
         <v>34</v>
@@ -4986,15 +4968,15 @@
         <v>6</v>
       </c>
       <c r="J119" s="9">
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="120" spans="1:10">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11">
       <c r="A120" t="s">
         <v>33</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="C120" t="s">
         <v>11</v>
@@ -5006,27 +4988,27 @@
         <v>12</v>
       </c>
       <c r="F120" s="10">
-        <v>2016</v>
+        <v>2020</v>
       </c>
       <c r="G120" t="s">
         <v>34</v>
       </c>
       <c r="H120" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I120">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J120" s="9">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="121" spans="1:10">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11">
       <c r="A121" t="s">
         <v>33</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="C121" t="s">
         <v>11</v>
@@ -5038,27 +5020,27 @@
         <v>12</v>
       </c>
       <c r="F121" s="10">
-        <v>2016</v>
+        <v>2020</v>
       </c>
       <c r="G121" t="s">
         <v>34</v>
       </c>
       <c r="H121" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I121">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J121" s="9">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="122" spans="1:10">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11">
       <c r="A122" t="s">
         <v>33</v>
       </c>
       <c r="B122" s="7" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="C122" t="s">
         <v>11</v>
@@ -5070,27 +5052,27 @@
         <v>12</v>
       </c>
       <c r="F122" s="10">
-        <v>2016</v>
+        <v>2020</v>
       </c>
       <c r="G122" t="s">
         <v>34</v>
       </c>
       <c r="H122" s="6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="I122">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J122" s="9">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="123" spans="1:10">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11">
       <c r="A123" t="s">
         <v>33</v>
       </c>
       <c r="B123" s="7" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="C123" t="s">
         <v>11</v>
@@ -5102,27 +5084,27 @@
         <v>12</v>
       </c>
       <c r="F123" s="10">
-        <v>2016</v>
+        <v>2020</v>
       </c>
       <c r="G123" t="s">
         <v>34</v>
       </c>
       <c r="H123" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I123">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J123" s="9">
-        <v>0.17</v>
-      </c>
-    </row>
-    <row r="124" spans="1:10">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11">
       <c r="A124" t="s">
         <v>33</v>
       </c>
       <c r="B124" s="7" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="C124" t="s">
         <v>11</v>
@@ -5134,7 +5116,7 @@
         <v>12</v>
       </c>
       <c r="F124" s="10">
-        <v>2016</v>
+        <v>2020</v>
       </c>
       <c r="G124" t="s">
         <v>34</v>
@@ -5149,7 +5131,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="125" spans="1:10">
+    <row r="125" spans="1:11">
       <c r="A125" t="s">
         <v>33</v>
       </c>
@@ -5166,7 +5148,7 @@
         <v>12</v>
       </c>
       <c r="F125" s="10">
-        <v>2016</v>
+        <v>2022</v>
       </c>
       <c r="G125" t="s">
         <v>34</v>
@@ -5178,10 +5160,13 @@
         <v>6</v>
       </c>
       <c r="J125" s="9">
-        <v>0.13</v>
-      </c>
-    </row>
-    <row r="126" spans="1:10">
+        <v>0.18</v>
+      </c>
+      <c r="K125">
+        <v>1544</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11">
       <c r="A126" t="s">
         <v>33</v>
       </c>
@@ -5198,22 +5183,25 @@
         <v>12</v>
       </c>
       <c r="F126" s="10">
-        <v>2016</v>
+        <v>2022</v>
       </c>
       <c r="G126" t="s">
         <v>34</v>
       </c>
       <c r="H126" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I126">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J126" s="9">
-        <v>0.14000000000000001</v>
-      </c>
-    </row>
-    <row r="127" spans="1:10">
+        <v>0.22</v>
+      </c>
+      <c r="K126">
+        <v>1891</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11">
       <c r="A127" t="s">
         <v>33</v>
       </c>
@@ -5230,22 +5218,25 @@
         <v>12</v>
       </c>
       <c r="F127" s="10">
-        <v>2016</v>
+        <v>2022</v>
       </c>
       <c r="G127" t="s">
         <v>34</v>
       </c>
       <c r="H127" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I127">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J127" s="9">
-        <v>0.21</v>
-      </c>
-    </row>
-    <row r="128" spans="1:10">
+        <v>0.13</v>
+      </c>
+      <c r="K127">
+        <v>1141</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11">
       <c r="A128" t="s">
         <v>33</v>
       </c>
@@ -5262,22 +5253,25 @@
         <v>12</v>
       </c>
       <c r="F128" s="10">
-        <v>2016</v>
+        <v>2022</v>
       </c>
       <c r="G128" t="s">
         <v>34</v>
       </c>
       <c r="H128" s="6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="I128">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J128" s="9">
         <v>0.17</v>
       </c>
-    </row>
-    <row r="129" spans="1:10">
+      <c r="K128">
+        <v>1480</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11">
       <c r="A129" t="s">
         <v>33</v>
       </c>
@@ -5294,22 +5288,25 @@
         <v>12</v>
       </c>
       <c r="F129" s="10">
-        <v>2016</v>
+        <v>2022</v>
       </c>
       <c r="G129" t="s">
         <v>34</v>
       </c>
       <c r="H129" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I129">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J129" s="9">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="130" spans="1:10">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="K129">
+        <v>1181</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11">
       <c r="A130" t="s">
         <v>33</v>
       </c>
@@ -5326,24 +5323,30 @@
         <v>12</v>
       </c>
       <c r="F130" s="10">
-        <v>2016</v>
+        <v>2022</v>
       </c>
       <c r="G130" t="s">
         <v>34</v>
       </c>
       <c r="H130" s="6" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="I130">
         <v>1</v>
       </c>
       <c r="J130" s="9">
-        <v>0.2</v>
+        <v>0.15</v>
+      </c>
+      <c r="K130">
+        <v>1280</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K76">
-    <sortCondition ref="H2:H76"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K131">
+    <sortCondition ref="A2:A131"/>
+    <sortCondition ref="B2:B131"/>
+    <sortCondition ref="F2:F131"/>
+    <sortCondition ref="H2:H131"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>